<commit_message>
json and report file removed
</commit_message>
<xml_diff>
--- a/DataBag/test_xlx.xlsx
+++ b/DataBag/test_xlx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev_Progs\cyanconnode_api_project\DataBag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BACC053-D123-4567-92BB-9A9BD2ACD05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBADD023-DE6E-46CC-80DB-80011E02068B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>status</t>
   </si>
   <si>
-    <t>dtttdddtreev1@gmail.com</t>
+    <t>dttsssev1@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>